<commit_message>
Add new wall assets and update image header
- Introduced new wall assets: mid-right.xpm, mid.xpm, single-bottom.xpm, single-mid.png, single-mid.xpm, single-top.xpm, top-left.xpm, top-right.xpm, top.xpm.
- Updated images.h to include paths for new wall assets.
- Ensured all new assets are properly defined and accessible within the project structure.
</commit_message>
<xml_diff>
--- a/_Notes/examples.xlsx
+++ b/_Notes/examples.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\simon\so_long\_Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8318F68-D622-4FD8-9453-DCA7550D2BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED2AF23-CE7E-4033-AF2F-46917F6BFBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="525" windowWidth="15285" windowHeight="11100" activeTab="1" xr2:uid="{E07D4DD8-0D98-4708-B0F0-44D58929705A}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{E07D4DD8-0D98-4708-B0F0-44D58929705A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
     <sheet name="map samples" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1 (3)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="19">
   <si>
     <t>E</t>
   </si>
@@ -67,6 +68,33 @@
   </si>
   <si>
     <t>Find 1st C: 1st C is closest to player</t>
+  </si>
+  <si>
+    <t>tile_size</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -110,11 +138,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -125,7 +150,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="20">
     <dxf>
       <font>
         <color theme="2"/>
@@ -221,6 +246,16 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2"/>
@@ -229,21 +264,78 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="2"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="5"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="2"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -577,58 +669,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC0BC44-EAC2-4023-8424-064219A611AD}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:AG41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13:AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="13" width="4" style="2"/>
+    <col min="2" max="13" width="4" style="1"/>
     <col min="17" max="17" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="3">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>4</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>5</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>6</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>7</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>8</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>9</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>10</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -667,237 +759,438 @@
       <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2">
+        <v>48</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W4" s="1">
+        <v>0</v>
+      </c>
+      <c r="X4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W5" s="1">
+        <v>0</v>
+      </c>
+      <c r="X5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W6" s="1">
+        <v>0</v>
+      </c>
+      <c r="X6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-      <c r="M5" s="1">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
-        <v>0</v>
-      </c>
-      <c r="L6" s="1">
-        <v>0</v>
-      </c>
-      <c r="M6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
@@ -934,9 +1227,45 @@
       <c r="M8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="V8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W8" s="1">
+        <v>0</v>
+      </c>
+      <c r="X8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="1">
@@ -975,9 +1304,45 @@
       <c r="M9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="V9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+      <c r="X9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -1016,9 +1381,45 @@
       <c r="M10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="V10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="1">
@@ -1057,9 +1458,45 @@
       <c r="M11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="V11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -1098,9 +1535,45 @@
       <c r="M12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="V12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="1">
@@ -1139,8 +1612,44 @@
       <c r="M13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>1</v>
       </c>
@@ -2054,14 +2563,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:M1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="C">
+    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",B2)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="E">
+      <formula>NOT(ISERROR(SEARCH("E",B2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V2:AG13">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",V2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",V2)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="E">
-      <formula>NOT(ISERROR(SEARCH("E",B2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("E",V2)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>0</formula>
@@ -2077,58 +2603,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38AF9D1E-6F50-4D6E-9B74-0B6A2CD0F5B0}">
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="13" width="4" style="2"/>
+    <col min="2" max="13" width="4" style="1"/>
     <col min="17" max="17" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="3">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3">
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
         <v>2</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1" s="2">
         <v>3</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1" s="2">
         <v>4</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="2">
         <v>5</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="2">
         <v>6</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I1" s="2">
         <v>7</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J1" s="2">
         <v>8</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1" s="2">
         <v>9</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L1" s="2">
         <v>10</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M1" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="1">
@@ -2172,7 +2698,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -2219,7 +2745,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -2266,7 +2792,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -2313,7 +2839,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="1">
@@ -2354,7 +2880,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -2398,7 +2924,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="1">
@@ -2442,7 +2968,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="1">
@@ -2486,7 +3012,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="1">
@@ -2527,7 +3053,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="1">
@@ -2568,7 +3094,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
       <c r="B12" s="1">
@@ -2609,7 +3135,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
       <c r="B13" s="1">
@@ -2650,45 +3176,45 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3">
+      <c r="B15" s="2">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
         <v>2</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>3</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>4</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="2">
         <v>5</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="2">
         <v>6</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>7</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>8</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="2">
         <v>9</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15" s="2">
         <v>10</v>
       </c>
-      <c r="M15" s="3">
+      <c r="M15" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>0</v>
       </c>
       <c r="B16" s="1">
@@ -2729,7 +3255,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="1">
@@ -2770,7 +3296,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>2</v>
       </c>
       <c r="B18" s="1">
@@ -2811,7 +3337,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
       <c r="B19" s="1">
@@ -2852,7 +3378,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>4</v>
       </c>
       <c r="B20" s="1">
@@ -2893,7 +3419,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>5</v>
       </c>
       <c r="B21" s="1">
@@ -2934,7 +3460,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>6</v>
       </c>
       <c r="B22" s="1">
@@ -2975,7 +3501,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>7</v>
       </c>
       <c r="B23" s="1">
@@ -3016,7 +3542,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>8</v>
       </c>
       <c r="B24" s="1">
@@ -3057,7 +3583,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>9</v>
       </c>
       <c r="B25" s="1">
@@ -3098,7 +3624,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>10</v>
       </c>
       <c r="B26" s="1">
@@ -3139,7 +3665,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>11</v>
       </c>
       <c r="B27" s="1">
@@ -3178,177 +3704,1509 @@
       <c r="M27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:M14 B16:M1048576">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="C">
+      <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="E">
+      <formula>NOT(ISERROR(SEARCH("E",B2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6391E796-5CB0-4884-8659-083AE38363EC}">
+  <dimension ref="A1:Q41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="13" width="4" style="1"/>
+    <col min="17" max="17" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1</v>
+      </c>
+      <c r="M13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>1</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+      <c r="M23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
+        <v>1</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>1</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>1</v>
+      </c>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1</v>
+      </c>
+      <c r="M30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>1</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1">
+        <v>1</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1">
+        <v>1</v>
+      </c>
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>1</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" s="1">
+        <v>1</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
+      <c r="K35" s="1">
+        <v>1</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+      <c r="M35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <v>0</v>
+      </c>
+      <c r="M36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1</v>
+      </c>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1">
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1">
+        <v>1</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0</v>
+      </c>
+      <c r="M37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <v>0</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
+        <v>0</v>
+      </c>
+      <c r="M38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+      <c r="I39" s="1">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1</v>
+      </c>
+      <c r="K39" s="1">
+        <v>1</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
+      </c>
+      <c r="M39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1">
+        <v>0</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
+      </c>
+      <c r="I41" s="1">
+        <v>1</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1</v>
+      </c>
+      <c r="K41" s="1">
+        <v>1</v>
+      </c>
+      <c r="L41" s="1">
+        <v>1</v>
+      </c>
+      <c r="M41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:M1048576">
     <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH("C",B2)))</formula>
     </cfRule>

</xml_diff>